<commit_message>
Vanilla Recycling Expanded 업데이트
쓰레기 바닥 추가
</commit_message>
<xml_diff>
--- a/Data/Vanilla Expanded/Vanilla Recycling Expanded - 3155781848/3155781848.xlsx
+++ b/Data/Vanilla Expanded/Vanilla Recycling Expanded - 3155781848/3155781848.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\240122\Vanilla Recycling Expanded - 3155781848\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.5.3\Vanilla Recycling Expanded - 3155781848\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADB50F8-5333-482C-915F-C9AE23DB869E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EE64A6-ED42-4E56-974D-12BBD24DECE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240209" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_240312" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -82,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G76" authorId="0" shapeId="0" xr:uid="{494928E4-E591-4624-90E3-345E62BE2479}">
+    <comment ref="G78" authorId="0" shapeId="0" xr:uid="{494928E4-E591-4624-90E3-345E62BE2479}">
       <text>
         <r>
           <rPr>
@@ -340,7 +353,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G77" authorId="0" shapeId="0" xr:uid="{304F5C7F-41E2-4B8B-B983-1D19C6B02933}">
+    <comment ref="G79" authorId="0" shapeId="0" xr:uid="{304F5C7F-41E2-4B8B-B983-1D19C6B02933}">
       <text>
         <r>
           <rPr>
@@ -412,7 +425,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="314">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1397,7 +1410,37 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>독성이 없는 일반 쓰레기를 압축하여 벽돌 모양으로 찍어낸 것입니다. 표면을 열로 처리하여 내구성을 높였습니다.\n\n벽을 세우거나 가구를 만드는 데 사용할 만큼 충분히 튼튼한 데다, 야외에 보관하더라도 석재처럼 자연적으로 손상되지 않습니다. 그러나 손상을 입을 때마다 상당량의 독소 가스를 방출합니다.</t>
+    <t>VRecyclingE_TrashBrickFloor.description</t>
+  </si>
+  <si>
+    <t>TerrainDef</t>
+  </si>
+  <si>
+    <t>TerrainDef+VRecyclingE_TrashBrickFloor.description</t>
+  </si>
+  <si>
+    <t>trashbrick floor</t>
+  </si>
+  <si>
+    <t>VRecyclingE_TrashBrickFloor.label</t>
+  </si>
+  <si>
+    <t>TerrainDef+VRecyclingE_TrashBrickFloor.label</t>
+  </si>
+  <si>
+    <t>쓰레기 바닥</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>독성이 없는 일반 쓰레기를 압축하여 벽돌 모양으로 찍어낸 것입니다. 표면을 열로 처리하여 내구성을 높였습니다.\n\n벽을 세우거나 가구를 만드는 데 사용할 만큼 충분히 튼튼한 데다, 야외에 보관하더라도 석재와 같이 자연적으로 손상되지 않습니다. 그러나 손상을 입을 때마다 상당량의 독소 가스를 방출합니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>A rough floor made with trashbricks. Not pretty, but cheap to make.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>압축 쓰레기를 깔아 만든 거친 바닥입니다. 보기엔 좀 그렇지만 싸게 만들 수 있습니다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1405,7 +1448,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1461,6 +1504,14 @@
       <name val="돋움"/>
       <family val="3"/>
       <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1605,7 +1656,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1619,6 +1670,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="메모" xfId="3" builtinId="10"/>
@@ -1924,10 +1976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1936,7 +1988,7 @@
     <col min="2" max="2" width="23.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.26953125" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="48.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="92.81640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="79.7265625" style="1" customWidth="1"/>
     <col min="7" max="7" width="36.90625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.1796875" style="1"/>
@@ -2412,884 +2464,919 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F30" s="7" t="s">
         <v>240</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F40" s="6" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="1" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="B41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="1" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="B42" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="F42" s="7" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="2" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B43" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2" t="s">
+      <c r="D43" s="2"/>
+      <c r="E43" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F43" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="3" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="B44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3" t="s">
+      <c r="D44" s="3"/>
+      <c r="E44" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="1" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="B45" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="F45" s="7" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A44" s="1" t="s">
+    <row r="46" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A46" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="B46" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F46" s="7" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="3" t="s">
+    <row r="47" spans="1:6" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="B47" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3" t="s">
+      <c r="D47" s="3"/>
+      <c r="E47" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F45" s="9"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="1" t="s">
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="B48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="F48" s="7" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="1" t="s">
+    <row r="49" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A49" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="B49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F49" s="7" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="3" t="s">
+    <row r="50" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="3" t="s">
+      <c r="B50" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3" t="s">
+      <c r="D50" s="3"/>
+      <c r="E50" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F48" s="9"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A49" s="1" t="s">
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A51" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="B51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F49" s="7" t="s">
+      <c r="F51" s="7" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A50" s="1" t="s">
+    <row r="52" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A52" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="B52" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="F52" s="7" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="3" t="s">
+    <row r="53" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C51" s="3" t="s">
+      <c r="B53" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3" t="s">
+      <c r="D53" s="3"/>
+      <c r="E53" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F51" s="9"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A52" s="1" t="s">
+      <c r="F53" s="9"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A54" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="B54" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="F52" s="7" t="s">
+      <c r="F54" s="7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A53" s="1" t="s">
+    <row r="55" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A55" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="B55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F55" s="7" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="3" t="s">
+    <row r="56" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C54" s="3" t="s">
+      <c r="B56" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3" t="s">
+      <c r="D56" s="3"/>
+      <c r="E56" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="F54" s="9"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A55" s="1" t="s">
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A57" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="B57" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F55" s="7" t="s">
+      <c r="F57" s="7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="1" t="s">
+    <row r="58" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A58" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="B58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F56" s="7" t="s">
+      <c r="F58" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="G58" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="3" t="s">
+    <row r="59" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C57" s="3" t="s">
+      <c r="B59" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3" t="s">
+      <c r="D59" s="3"/>
+      <c r="E59" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="F57" s="9"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A58" s="1" t="s">
+      <c r="F59" s="9"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A60" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="B60" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F58" s="7" t="s">
+      <c r="F60" s="7" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="1" t="s">
+    <row r="61" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A61" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C59" s="1" t="s">
+      <c r="B61" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F59" s="7" t="s">
+      <c r="F61" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="G61" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="3" t="s">
+    <row r="62" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C60" s="3" t="s">
+      <c r="B62" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3" t="s">
+      <c r="D62" s="3"/>
+      <c r="E62" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="F60" s="9"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A61" s="1" t="s">
+      <c r="F62" s="9"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A63" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C61" s="1" t="s">
+      <c r="B63" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A62" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="G62" s="8" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A63" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>186</v>
       </c>
       <c r="F63" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A64" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A65" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="G63" s="8" t="s">
+      <c r="G65" s="8" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="3" t="s">
+    <row r="66" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A66" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C64" s="3" t="s">
+      <c r="B66" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3" t="s">
+      <c r="D66" s="3"/>
+      <c r="E66" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="F64" s="9"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A65" s="1" t="s">
+      <c r="F66" s="9"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A67" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F67" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="G65" s="8" t="s">
+      <c r="G67" s="8" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A66" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A67" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>193</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A69" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A70" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E70" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F68" s="7" t="s">
+      <c r="F70" s="7" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A69" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A70" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>193</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A72" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A73" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E73" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F71" s="7" t="s">
+      <c r="F73" s="7" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A72" s="1" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A74" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E74" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A73" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="G73" s="8" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A74" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B74" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="D74" s="10"/>
-      <c r="E74" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="F74" s="10"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="F75" s="12" t="s">
-        <v>260</v>
+        <v>217</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>294</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>261</v>
+        <v>282</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A76" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B76" s="1" t="s">
+      <c r="A76" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B76" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="G76" s="8" t="s">
-        <v>292</v>
-      </c>
+      <c r="C76" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F76" s="10"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F77" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="G77" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A78" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="G78" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A79" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="F77" s="12" t="s">
+      <c r="F79" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="G77" s="8" t="s">
+      <c r="G79" s="8" t="s">
         <v>292</v>
       </c>
     </row>

</xml_diff>